<commit_message>
modif sur mon dossier perso
</commit_message>
<xml_diff>
--- a/BDD/Tests/ProcesVerbaux/Proces_PEA_verifierAccesBadge.xlsx
+++ b/BDD/Tests/ProcesVerbaux/Proces_PEA_verifierAccesBadge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopti\Documents\Projet\BDD\Tests\ProcesVerbaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE22973-9876-40CF-86A7-01350DB6D62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E20D121-3CBC-467B-BC69-789D00BCA80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>Environnement du test</t>
   </si>
   <si>
-    <t>API en marche</t>
-  </si>
-  <si>
     <t>Procédure du test</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Le test est réalisé sur une machine virtuelle Debian 12 à du fichier pytest verifierAccesBadge.py.</t>
+  </si>
+  <si>
+    <t>Pytest installé</t>
   </si>
 </sst>
 </file>
@@ -254,53 +254,53 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -586,7 +586,7 @@
   <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,216 +597,216 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>45728</v>
+      </c>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="2:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+    </row>
+    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="2:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>45728</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="2:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="2:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B18" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B21" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>